<commit_message>
Consertei espacos entre emojis
</commit_message>
<xml_diff>
--- a/PS5.xlsx
+++ b/PS5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agchi\Documents\GitHub\P1-Ciencia-dos-Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661C4900-AF16-4E37-A0DD-3B7E9664FDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99AB76-F88C-4CA7-AD99-54FBC1F20616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4635" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="729">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1874,15 +1874,9 @@
     <t>@meuplaystation flw galeraaaaa vou lá no estados unidos compro 4 ps5 7 pc gamer 2 xbox quando voltar eu vou vender por 30000</t>
   </si>
   <si>
-    <t>evento da sony amanhã vai ter- god of war ragnarok- bloodborne 2- elden ring- silent hills - preços do ps5fontes quentes confirmaram 🙌🏼</t>
-  </si>
-  <si>
     <t>acordei né de boa fui na cozinha tomar um café e minha sobrinha veio me dar bom dia dei logo um chutão joguei ela na porta bom dia é o caralho hoje é dia ps5 silent hill finalmente preço e data dessa porra gameplays jogos fodas. que mané bom dia. #ps5showcase #ps5</t>
   </si>
   <si>
-    <t>imagina pra consumir ps5 ano que vem  mais jogos e produtos eletronicos   com nossa moeda desvalorizada  pessima noticia  https//t.co/9qpmmhp5qo</t>
-  </si>
-  <si>
     <t>primeiro a nintendo fecha as portas no brasil agora a sony. preparem-se para os preços nada convidativos dos modelos do ps5</t>
   </si>
   <si>
@@ -1898,9 +1892,6 @@
     <t>discord https//t.co/q6oxummoxfsiga nossas midias sociais e acompanhe memes noticias vídeos e lives @aldoriagamesseja apoiador e participe de sorteios#memes #humor #meme #nostalgia #ps5 #ps4 #xbox https//t.co/1xors1usty</t>
   </si>
   <si>
-    <t>é hoje 😱⌛️😱⌛️gostou do vídeo? compartilhenos siga em todas as redes sociais só pesquisar por #playfivebrasil no instagram e facebook#ps5 #ps5showcase #playstation #game #sony @sony @sonybrasil @playstation @playstation_br https//t.co/d1fzxdlwn5</t>
-  </si>
-  <si>
     <t>as maiores e persistentes dúvidas sobre a ps5 a que a sony precisa dar resposta no showcase de mais logo. https//t.co/gvu0ajt5lg</t>
   </si>
   <si>
@@ -1910,30 +1901,15 @@
     <t>se a sony botar o lançamento do ps5 em novembro também vocês já sabem o que me dar de aniversário né??</t>
   </si>
   <si>
-    <t>está chegando a hora 17h tem o grande evento do ano até o momento. meu palpite para o ps5 é de €49990 com leitor.€39990 sem leitor.  https//t.co/yjmbnerwjv</t>
-  </si>
-  <si>
     <t>@breninhoo19 @mikkaizinho @mitodante_ eu não botei defeito nenhum eu acho playstation sensacional eu não tenho guerra de console mas o ps5 é inferior que o xbox series x</t>
   </si>
   <si>
     <t>e meu priminho que sabia que eu ia ficar nervosa com a cirurgia do stark e me mandou o ps5 dele pra eu relaxa 💜</t>
   </si>
   <si>
-    <t>@capitaocritica mano pra que fica de boa jogando o seu ps5 que eu fico deboa no xbox 🙂👍</t>
-  </si>
-  <si>
     <t>bom dia hoje tem precinho do ps5 será?</t>
   </si>
   <si>
-    <t>amanhã tem evento da sony sobre o ps5. a capcom já confirmou que as tão esperadas novidades de #revillage chegam no fim de setembromas será que amanhã a gente pode ter algo novo? nem que seja uma nova imagem? 👀#rebhfun https//t.co/fto9ghdlai</t>
-  </si>
-  <si>
-    <t>é hoje 🤍🖤💙 #ps5showcase #ps5 https//t.co/ejjqhjnfgg</t>
-  </si>
-  <si>
-    <t>@cariocachinese @gmunhoz__ negócio é esperar lançar ps5 pra comprar o 4 e assim vai indo os com o xbox também pq da muito stönks 🤏😎👍</t>
-  </si>
-  <si>
     <t>sinceramente meu hype pro evento do ps5 é preço e data de lançamento só isso não espero nada demais além disso no máximo um trailer novo ou gameplay de jogos já apresentados.</t>
   </si>
   <si>
@@ -1982,21 +1958,9 @@
     <t>@kamatsukyoto a dos xbox tão bonitas pômas essa do ps5parece de cafeteira</t>
   </si>
   <si>
-    <t>#tlou2 😱já garantiu o seu #thelastofus2⁉veja este e outros grandes sucessos aqui na #bigboygames 😍aproveite pois são pouca unidades🏃🏃‍♀️https//t.co/jkwzknhfujcompramos seu jogo usado📱16 99763-7729#lojabigboygames #bigboy #ps4 #playstation4 #ps5 #seminovos https//t.co/tv8bfcgjgq</t>
-  </si>
-  <si>
     <t>@rjrmarafon @m4ximizando caraca véi independente de qualquer coisa o ps5 é enorme mesmo.</t>
   </si>
   <si>
-    <t>hoje também é dia de saber mais do #playstation5   o evento playstation 5 showcase acontece hoje às 17h do horário de brasília. quem aí tá animado pra saber mais do #ps5? https//t.co/zythhmpp5v</t>
-  </si>
-  <si>
-    <t>@dougmad4k des d quando o fechamento da fabrica devido a impostos alta do dolar etc tem com a venda elevada no preço do ps5 aki ja q a sony nao fabricava video game no território nacional .sera q alguem leu a materia sem falar q varias pessoas vao ficar sem emprego  mas bora comemorar</t>
-  </si>
-  <si>
-    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão  nessa porra e a ela vem com bom dia toma no cu https//t.co/tniofq4gtl</t>
-  </si>
-  <si>
     <t>@arielsis kabum vai sortear um ps5 no provável day one acho que isso já era indícios que seria lançado aqui day one</t>
   </si>
   <si>
@@ -2048,18 +2012,12 @@
     <t>jogar the last of us part ii no ps5 ou talvez um red dead redemption 2 já me dá um negócio. the witcher 3 então.vamo q hoje não é um dia qualquer#ps5#ps5showcase</t>
   </si>
   <si>
-    <t>palpites de hoje us 449 / 499   br 5999 / 6499#ps5</t>
-  </si>
-  <si>
     <t>personagem memorável e incrível do mundo os gamesobs espero que o evento do ps5 hoje ao menos tenhamos mais informações sobre datas dos jogos e claro a data e preço do ps5bom dia a todos os sonysta/a todos que amam vídeo game. https//t.co/ooflly63nj</t>
   </si>
   <si>
     <t>@porraissaa so uma tunada naquele pc um ps5 do lado com um monitor 4k puts ai eu quero</t>
   </si>
   <si>
-    <t>o evento do ps5 vai começar quando eu tiver largando  se aparecer algo de algum final fantasy metam minha @ no post por favor</t>
-  </si>
-  <si>
     <t>fiquem em casa a economia vemos depois.depoister que vender a casa para comprar o ps5 https//t.co/khjmw47bxs</t>
   </si>
   <si>
@@ -2078,18 +2036,12 @@
     <t>acordei agr n consigo mais dormir n to hypadona pro evento do ps5 meo deos https//t.co/svdf9s6oa5</t>
   </si>
   <si>
-    <t>vamos lá.. hoje é  o dia dos anúncios do ps5 qual você acha que será o preço?eu acredito em 599 com disco e 499 para a versão sem disco.</t>
-  </si>
-  <si>
     <t>@cooperfsss demons souls no dia do lançamento??? será? esse é o que eu acho mais dificil das coisas que tenho visto. acredito mais no ffxvi como exclusivo de ps5</t>
   </si>
   <si>
     <t>teremos xbox series x e series s no brasil no day one. o país cresceu ainda mais na indústria nos últimos anos e foi notado pelas duas grandes empresas.créditos mais uma vez ao @silva_ruancarlo que já havia informado sobre o #ps5 https//t.co/jaeqn65mfv</t>
   </si>
   <si>
-    <t>liberal/anarco de facebook ain sou contra o protecionismo à indústriasony vou sairl/a  a culpa é sua seus comunistaaaaasl/a  e meu ps5? paieeee</t>
-  </si>
-  <si>
     <t>@ikarojyo_ na verdade isso não afeta o ps5a sony já não produz console aqui desde 2017. mas é um péssimo sinal para a economia do brasil</t>
   </si>
   <si>
@@ -2102,9 +2054,6 @@
     <t>@obitouc84502465 @there4lon3 @shazamcaraiu @artlocked @isadorabasile pera tu ta falando pra ele comprar um ps5 mas dps fala q a comunidade de ps é suja n to entendendo porra nenhuma</t>
   </si>
   <si>
-    <t>vazou as primeiras imagens de the last of us part 3 no ps5 que a sony vai mostrar no evento de hoje. 🗣️🚨🚨🚨🚨🚨🚨🚨🚨 https//t.co/adpp6gn7yi</t>
-  </si>
-  <si>
     <t>que o preço do ps5 saia amanhã amém</t>
   </si>
   <si>
@@ -2114,18 +2063,12 @@
     <t>semana agitada com conferência do ps5 hoje e possível preço se não mostrar hoje será “preço inbox” amanhã tem direct mini da nintendo com possível monster hunter e sexta nova apresentação de novidades do cyberpunk 2077.</t>
   </si>
   <si>
-    <t>nesse evento do ps5 amanhã a santa monica poderia anunciar algum teaser sobre uma continuação do god of war hein🤔</t>
-  </si>
-  <si>
     <t>@afrobaiano haha claro bem as pessoas são livres para sentir o que quiser ação / consequência némas eu não vejo desmérito na fala tanto que a palavra liquidação quem disse foi você nétodo mundo quer um ps5 nem por isso tá na liquidação</t>
   </si>
   <si>
     <t>@lfernando912 a sony teve que descartar 4 milhões de processadores de ps5 essa semana será que derreteram quando o ps5 bateu os 10 teraflops com o overclock durante o teste de qualidade?</t>
   </si>
   <si>
-    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão  nessa porra e a ela vem com bom dia toma no cu https//t.co/e04w0wqxyc</t>
-  </si>
-  <si>
     <t>é hoje o velório e sepultamento do xbox. finalmente acaba a espera pela revelação oficial do preço do ps5. se o dólar maldito colaborar eu compro a versão sem leitor de mídia física ainda em 2020 via mercado cinza. https//t.co/lw5gfkkrsr</t>
   </si>
   <si>
@@ -2144,30 +2087,18 @@
     <t>timeline hojevem ni mim #ps5 https//t.co/cde1na405h</t>
   </si>
   <si>
-    <t>conhecendo o mercenarismo da sony não duvido nada que esse ps5 digital edition seja anunciado mais tarde por uns 500 dols espero quebrar a cara 🙏🏼</t>
-  </si>
-  <si>
     <t>lembrando que hoje é o dia do ps5. vamos ver</t>
   </si>
   <si>
     <t>vamo de xbox ou ps5 nessa gen hein eita duvida</t>
   </si>
   <si>
-    <t>que hoje é dia de #ps5showcase o mundo todo sabe e está de olho 👀uma das apostas para o evento de hoje é que o @playstation @playstation_br mostre sua nova interface em funcionamentoa tela de boot a gente já conhece será que veremos tudo hoje? façam suas apostas #ps5 https//t.co/zmrprtjv1t</t>
-  </si>
-  <si>
     <t>@xzticks @maisxbox pior do piorpra cada coisa que ela falar que o ps5 tem e o xss não tem eu falo 3 coisas que o xss tem e o ps5 não tem.</t>
   </si>
   <si>
     <t>pqp tl muito ansioso para o novo evento do ps5 krl#ps5showcase #ps5</t>
   </si>
   <si>
-    <t>será que hoje teremos novidades? 🥰🥰🥰 #ps5 #ps5showcase https//t.co/3lgnv7jofi</t>
-  </si>
-  <si>
-    <t>→ sony realiza evento do playstation 5 nesta quarta 👉🏻 #tech #games #ps5 #playstation5 #sony #jornaldoscanyons #jdc🔗 confira no jornal dos canyons https//t.co/c5ioiz4jhb</t>
-  </si>
-  <si>
     <t>eu não podia deixar de soltar isso um vídeo pra vcs da nossa reação ao trailer de anúncio do spider-man miles morales no evento de revelação do #ps5quem puder curtir compartilhar e se inscrever no canal vai ajudar demaishttps//t.co/4wgd3czrur https//t.co/1pai5sqjks</t>
   </si>
   <si>
@@ -2183,9 +2114,6 @@
     <t>acordei né e tals aí fui na cozinha tomar um café e minha sobrinha veio correndo me abraçar pra me dar bom dia dei logo um chutão joguei na porta bom dia o caralho hoje é dia de guerra porradia de apresentar o #ps5 mané bom dia pilhadão e a criança vem me da bom dia? kkk</t>
   </si>
   <si>
-    <t>agenda ai pra acompanhar comigo https//t.co/zwkgfqbczjaposto   ps5 com leitor  44900 $  sem leitor  34900 $#playstation5 #playstation5preço #ps5reveal #ps5showcase #playstation5showcase #ps5preço #playstation5preço</t>
-  </si>
-  <si>
     <t>será que teremos novidades? #ps5 #ps5showcase https//t.co/opy5camouh</t>
   </si>
   <si>
@@ -2198,9 +2126,6 @@
     <t>@matheus_luzzz então é sobre isso mesmo.. faz a regra de três em cima desse valor da 3080. vamos supor que o ps5 seja 70% dessa placa. ficaria perto dos 4k. será ??</t>
   </si>
   <si>
-    <t>- imran khan puta merda o series x tem 98 libras 4.5kg é mais pesado que um bebê recém-nascido- kez meu irmão tinha 14 libras 6.3kg 😬 quando nasceusó falando - timdog  isso é o quanto pesa o ps5pessoal veio reclamar do peso do series x 🤣🤣🤣 6kg e 300g 🤣🤣 https//t.co/o3qo85ugok</t>
-  </si>
-  <si>
     <t>a sony saindo do país o dólar altomeu ps5 cada vez mais longe</t>
   </si>
   <si>
@@ -2210,9 +2135,6 @@
     <t>deus que me perdoe mas se o ps5 chegar abaixo de 5k vou compra-lo no lançamento</t>
   </si>
   <si>
-    <t>ps5  custando o cheque do queiroz pra michelle. https//t.co/lopot8tsep</t>
-  </si>
-  <si>
     <t>venha a nós a ps5 🤩 https//t.co/aszd9crxuq</t>
   </si>
   <si>
@@ -2228,24 +2150,15 @@
     <t>@brayan20081448 @of_zenon @fazeclan @fakie @fazeblaze @fazesway cz c tá passando vergonha kkkkkk ele fez pq ele qr ter um futuro e vc tá zoando isso agr tu mal sabe que pra aumentar o fps teriam que criar um novo console que no caso e o ps5 https//t.co/4qwogsddgs</t>
   </si>
   <si>
-    <t>boooom diaaaaa a programação de hoje na nossa land será a seguinte às 14h30 vamos abrir nossa live normalmente para jogar um crash maroto. às 16h30 mais ou menos vamos invadir o canal do nosso parceiro @leongameplay01 para acompanharmos juntos o evento do ps5. conto com vcs🤓 https//t.co/lhfdv87jgb</t>
-  </si>
-  <si>
     <t>@guilherme_jarb ps5 dá chulé</t>
   </si>
   <si>
     <t>tenis chegou vai todo mundo tomarno cu bom dia primeiramente eu quero que caixista chore bem muito hoje pra eu beber as lágrimas ps5 vai botar pra mamar</t>
   </si>
   <si>
-    <t>hoje tem evento do ps5😎✌✌👍👍👍👍👍👍 https//t.co/jafc2avlrp</t>
-  </si>
-  <si>
     <t>👍 on @youtube sony vai fechar fábrica no brasil | seg. a bloomberg sony esta com problemas no processador do ps5 https//t.co/tof8qbstzm</t>
   </si>
   <si>
-    <t>é hoje 🎮sai o preço do ps5 pra baixar o preço do ps4 ps3 ficar em conta o ps2 a preço de banana pra eu poder pegar um ps1 usado. #ps5showcase</t>
-  </si>
-  <si>
     <t>ps5 sony nega mudanças na linha de produção após rumores de problemas com chipshttps//t.co/lisnce0e2w #tech #sony</t>
   </si>
   <si>
@@ -2279,15 +2192,6 @@
     <t>@kamatsukyoto as do xbox ficaram ótimas quem sabe esse ano a sony ainda mostre a do ps5</t>
   </si>
   <si>
-    <t>se o xbox one s que é tido como o console mais fraco dessa geração consegue fazer isso aqui em tempo real imagina o ps5 e xbox series x 👁️ https//t.co/gwljpuerlm</t>
-  </si>
-  <si>
-    <t>reino dos magos #5 ps5 sorteioloja  https//t.co/psooztpdjt</t>
-  </si>
-  <si>
-    <t>é hoje que vamos ver se eu compro o ps5 ano que vem ou só em 2022 😂😂</t>
-  </si>
-  <si>
     <t>@silva_ruancarlo @tokyo_90l eles tem alguma noção de unidades que vão ser distribuidas para esses consoles xbox e ps5 ?</t>
   </si>
   <si>
@@ -2300,9 +2204,6 @@
     <t>terão que reduzir o preço do console na força do ódio para ter concorrência com o xbox. o consumidor agradece. rss #hojetem #ps5 https//t.co/ksvf7fydmx</t>
   </si>
   <si>
-    <t>vai quenão custa sonhar né? 😆😆#ps5 #ps5showcase #playstation #playfivebrasil https//t.co/p7pjuultcq</t>
-  </si>
-  <si>
     <t>@locobaltar amanhã o dia é da mídia sonysta o poderoso ps5 vai mostrar o que é nova geração de verdade e se rolar o god of war novo podem enterrar a caixa preta da microsoft.</t>
   </si>
   <si>
@@ -2324,9 +2225,6 @@
     <t>@fazendachernoby ansioso demais pra ver as primeiras comparações gráficas entre series s e ps5. sim eu falei series s pra mim tá com cara que esse console base da ms vai dar pau no ps5. esperemos.</t>
   </si>
   <si>
-    <t>@gramiliki_ @nintendoamerica @rockstargames podia soltar aqele trailer de boyoneta 3 um zelda botw 2 e gta5   nao ligo para gta5 mas muito gente quer ele. pronto a nitnendo todo mundokkk. e no final mostra o suposto swtich prokkkkkkkkkk. pronto a nintendo ganhou o ano contra o ps5 e xbx ss x y z..kkkk</t>
-  </si>
-  <si>
     <t>isso aqui dá um comentário político daqueles você começaria com o engajamento alienado e reprodução de discursos na internet do consumidor imbecilizado nas novas mídias e chegaria na política econômica desastrosa do governo atual.https//t.co/mtndmtra12</t>
   </si>
   <si>
@@ -2336,12 +2234,6 @@
     <t>ps5 mais caro que um apartamento https//t.co/nl9mommvbc</t>
   </si>
   <si>
-    <t>@davidpdcoelho @xzticks @maisxbox só faltou ela falar não comprem o xss ps5 digital é melhor escolha. 😂😂😂</t>
-  </si>
-  <si>
-    <t>parabéns aos gamers apoiadores do bozo.sony brasil fechou sua fábrica em manaus o que obviamente impossibilitará fabricação nacional do ps5.tratem de pagar o meu agora.🖕🖕🖕🖕🖕🖕🖕🖕</t>
-  </si>
-  <si>
     <t>qualquer valor abaixo de 450/500 dolares hoje do ps5 é lucro. se for acima os caras vão ter q garantir nos jogos.#playstation5</t>
   </si>
   <si>
@@ -2363,9 +2255,6 @@
     <t>é hj o ps5 ?</t>
   </si>
   <si>
-    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão  nessa porra e a ela vem com bom dia toma no cu</t>
-  </si>
-  <si>
     <t>@rafapaulocr tomara q n seja só um anúncio dizendo que help wanted vai sair pra ps5 também se isso acontecer eu saio da live e vochora</t>
   </si>
   <si>
@@ -2432,21 +2321,9 @@
     <t>👍 on @youtube problematizando games #35 ps5 com defeito? 1440p maior que 4k? nvidia = skynet https//t.co/jndxfeudo7</t>
   </si>
   <si>
-    <t>@carlinhostroll no laçamento do ps4.. comprei de você  que ajudou vários gamers brasileiros  você podia vender novamente o xbox e ps5  em 🥺</t>
-  </si>
-  <si>
-    <t>já trouxe o terno da lavanderia. pro martini mexido e não batido tem tudo.mandei os cachorros pra casa da vó e as crianças pra pet 🤔🤔🤔.pedi divórcio entre 16h45 até 18h45. desfiz todas as amizades.hoje é dia de #ps5showcase #ps5</t>
-  </si>
-  <si>
     <t>preparados para vê o melhor exclusivo do ps5 no evento de amanhã #ps5 https//t.co/0x8lbmgwid</t>
   </si>
   <si>
-    <t>tomara que a rapaziada do xbox n venha pro ps5  tem uns q são chatão pqp</t>
-  </si>
-  <si>
-    <t>jogos que adoraria ver aparecendo amanhã na conferência do ps5 mas que obviamente vão permanecer só nos corações mesmo 😭👌 https//t.co/5qadryqu7v</t>
-  </si>
-  <si>
     <t>@lord_psmg lord acha possível aparecer god of war sillent hill ps now na américa latina e preço do ps5 mais barato?</t>
   </si>
   <si>
@@ -2475,6 +2352,156 @@
   </si>
   <si>
     <t>as vezes dá medo de pensar que o #ps5 chegue no brasil a menos de 5k.. eu cometeria uma loucura? talvez.</t>
+  </si>
+  <si>
+    <t>evento da sony amanhã vai ter- god of war ragnarok- bloodborne 2- elden ring- silent hills - preços do ps5fontes quentes confirmaram 🙌 🏼</t>
+  </si>
+  <si>
+    <t>imagina pra consumir ps5 ano que vem mais jogos e produtos eletronicos  com nossa moeda desvalorizada pessima noticia https//t.co/9qpmmhp5qo</t>
+  </si>
+  <si>
+    <t>é hoje 😱 ⌛ ️ 😱 ⌛ ️gostou do vídeo? compartilhenos siga em todas as redes sociais só pesquisar por #playfivebrasil no instagram e facebook#ps5 #ps5showcase #playstation #game #sony @sony @sonybrasil @playstation @playstation_br https//t.co/d1fzxdlwn5</t>
+  </si>
+  <si>
+    <t>está chegando a hora 17h tem o grande evento do ano até o momento. meu palpite para o ps5 é de €49990 com leitor.€39990 sem leitor. https//t.co/yjmbnerwjv</t>
+  </si>
+  <si>
+    <t>@capitaocritica mano pra que fica de boa jogando o seu ps5 que eu fico deboa no xbox 🙂 👍</t>
+  </si>
+  <si>
+    <t>amanhã tem evento da sony sobre o ps5. a capcom já confirmou que as tão esperadas novidades de #revillage chegam no fim de setembromas será que amanhã a gente pode ter algo novo? nem que seja uma nova imagem? 👀 #rebhfun https//t.co/fto9ghdlai</t>
+  </si>
+  <si>
+    <t>é hoje 🤍 🖤 💙 #ps5showcase #ps5 https//t.co/ejjqhjnfgg</t>
+  </si>
+  <si>
+    <t>@cariocachinese @gmunhoz__ negócio é esperar lançar ps5 pra comprar o 4 e assim vai indo os com o xbox também pq da muito stönks 🤏 😎 👍</t>
+  </si>
+  <si>
+    <t>@vingadorbrambz quem sabe é essa solução para super aquecimento do ps5 🤣 🤣 🤣</t>
+  </si>
+  <si>
+    <t>#tlou2 😱 já garantiu o seu #thelastofus2 ⁉ veja este e outros grandes sucessos aqui na #bigboygames 😍 aproveite pois são pouca unidades 🏃 🏃 ‍ ♀ ️https//t.co/jkwzknhfujcompramos seu jogo usado 📱 16 99763-7729#lojabigboygames #bigboy #ps4 #playstation4 #ps5 #seminovos https//t.co/tv8bfcgjgq</t>
+  </si>
+  <si>
+    <t>@marqueszero boa sorte em resolver pepinos e tenhamos fé que o ps5 seja barato aqui no brasil 🙌 🏻 🙌 🏻 🙌 🏻 🙌 🏻</t>
+  </si>
+  <si>
+    <t>hoje também é dia de saber mais do #playstation5  o evento playstation 5 showcase acontece hoje às 17h do horário de brasília. quem aí tá animado pra saber mais do #ps5? https//t.co/zythhmpp5v</t>
+  </si>
+  <si>
+    <t>@dougmad4k des d quando o fechamento da fabrica devido a impostos alta do dolar etc tem com a venda elevada no preço do ps5 aki ja q a sony nao fabricava video game no território nacional .sera q alguem leu a materia sem falar q varias pessoas vao ficar sem emprego mas bora comemorar</t>
+  </si>
+  <si>
+    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão nessa porra e a ela vem com bom dia toma no cu https//t.co/tniofq4gtl</t>
+  </si>
+  <si>
+    <t>palpites de hoje us 449 / 499  br 5999 / 6499#ps5</t>
+  </si>
+  <si>
+    <t>o evento do ps5 vai começar quando eu tiver largando se aparecer algo de algum final fantasy metam minha @ no post por favor</t>
+  </si>
+  <si>
+    <t>vamos lá.. hoje é o dia dos anúncios do ps5 qual você acha que será o preço?eu acredito em 599 com disco e 499 para a versão sem disco.</t>
+  </si>
+  <si>
+    <t>liberal/anarco de facebook ain sou contra o protecionismo à indústriasony vou sairl/a a culpa é sua seus comunistaaaaasl/a e meu ps5? paieeee</t>
+  </si>
+  <si>
+    <t>vazou as primeiras imagens de the last of us part 3 no ps5 que a sony vai mostrar no evento de hoje. 🗣 ️ 🚨 🚨 🚨 🚨 🚨 🚨 🚨 🚨 https//t.co/adpp6gn7yi</t>
+  </si>
+  <si>
+    <t>nesse evento do ps5 amanhã a santa monica poderia anunciar algum teaser sobre uma continuação do god of war hein 🤔</t>
+  </si>
+  <si>
+    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão nessa porra e a ela vem com bom dia toma no cu https//t.co/e04w0wqxyc</t>
+  </si>
+  <si>
+    <t>conhecendo o mercenarismo da sony não duvido nada que esse ps5 digital edition seja anunciado mais tarde por uns 500 dols espero quebrar a cara 🙏 🏼</t>
+  </si>
+  <si>
+    <t>que hoje é dia de #ps5showcase o mundo todo sabe e está de olho 👀 uma das apostas para o evento de hoje é que o @playstation @playstation_br mostre sua nova interface em funcionamentoa tela de boot a gente já conhece será que veremos tudo hoje? façam suas apostas #ps5 https//t.co/zmrprtjv1t</t>
+  </si>
+  <si>
+    <t>será que hoje teremos novidades? 🥰 🥰 🥰 #ps5 #ps5showcase https//t.co/3lgnv7jofi</t>
+  </si>
+  <si>
+    <t>→ sony realiza evento do playstation 5 nesta quarta 👉 🏻 #tech #games #ps5 #playstation5 #sony #jornaldoscanyons #jdc 🔗 confira no jornal dos canyons https//t.co/c5ioiz4jhb</t>
+  </si>
+  <si>
+    <t>tô pensando em vender meu corsa pra comprar o ps5 🤣 🤣 🤣 🤣</t>
+  </si>
+  <si>
+    <t>trabalhar pra comprar meu ps5 ♥ ️</t>
+  </si>
+  <si>
+    <t>agenda ai pra acompanhar comigo https//t.co/zwkgfqbczjaposto  ps5 com leitor 44900 $ sem leitor 34900 $#playstation5 #playstation5preço #ps5reveal #ps5showcase #playstation5showcase #ps5preço #playstation5preço</t>
+  </si>
+  <si>
+    <t>meu amigo esse ps5 vai sair por 10 mil conto. pense numa bomba.</t>
+  </si>
+  <si>
+    <t>- imran khan puta merda o series x tem 98 libras 4.5kg é mais pesado que um bebê recém-nascido- kez meu irmão tinha 14 libras 6.3kg 😬 quando nasceusó falando - timdog isso é o quanto pesa o ps5pessoal veio reclamar do peso do series x 🤣 🤣 🤣 6kg e 300g 🤣 🤣 https//t.co/o3qo85ugok</t>
+  </si>
+  <si>
+    <t>ps5 custando o cheque do queiroz pra michelle. https//t.co/lopot8tsep</t>
+  </si>
+  <si>
+    <t>boooom diaaaaa a programação de hoje na nossa land será a seguinte às 14h30 vamos abrir nossa live normalmente para jogar um crash maroto. às 16h30 mais ou menos vamos invadir o canal do nosso parceiro @leongameplay01 para acompanharmos juntos o evento do ps5. conto com vcs 🤓 https//t.co/lhfdv87jgb</t>
+  </si>
+  <si>
+    <t>hoje tem evento do ps5 😎 ✌ ✌ 👍 👍 👍 👍 👍 👍 https//t.co/jafc2avlrp</t>
+  </si>
+  <si>
+    <t>é hoje 🎮 sai o preço do ps5 pra baixar o preço do ps4 ps3 ficar em conta o ps2 a preço de banana pra eu poder pegar um ps1 usado. #ps5showcase</t>
+  </si>
+  <si>
+    <t>@voxeloficial imagina se fosse o #ps5 iria chover 🐑 pra comemorar tal notícia 🤣 🤣</t>
+  </si>
+  <si>
+    <t>se o xbox one s que é tido como o console mais fraco dessa geração consegue fazer isso aqui em tempo real imagina o ps5 e xbox series x 👁 ️ https//t.co/gwljpuerlm</t>
+  </si>
+  <si>
+    <t>reino dos magos #5 ps5 sorteioloja https//t.co/psooztpdjt</t>
+  </si>
+  <si>
+    <t>é hoje que vamos ver se eu compro o ps5 ano que vem ou só em 2022 😂 😂</t>
+  </si>
+  <si>
+    <t>vai quenão custa sonhar né? 😆 😆 #ps5 #ps5showcase #playstation #playfivebrasil https//t.co/p7pjuultcq</t>
+  </si>
+  <si>
+    <t>que hoje mostre mais de ps5 e seus jogos e esqueça de vez godfall 🙏 🏻</t>
+  </si>
+  <si>
+    <t>@gramiliki_ @nintendoamerica @rockstargames podia soltar aqele trailer de boyoneta 3 um zelda botw 2 e gta5  nao ligo para gta5 mas muito gente quer ele. pronto a nitnendo todo mundokkk. e no final mostra o suposto swtich prokkkkkkkkkk. pronto a nintendo ganhou o ano contra o ps5 e xbx ss x y z..kkkk</t>
+  </si>
+  <si>
+    <t>@davidpdcoelho @xzticks @maisxbox só faltou ela falar não comprem o xss ps5 digital é melhor escolha. 😂 😂 😂</t>
+  </si>
+  <si>
+    <t>parabéns aos gamers apoiadores do bozo.sony brasil fechou sua fábrica em manaus o que obviamente impossibilitará fabricação nacional do ps5.tratem de pagar o meu agora. 🖕 🖕 🖕 🖕 🖕 🖕 🖕 🖕</t>
+  </si>
+  <si>
+    <t>acordei né de boa fui na cozinha tomar café e minha irmã veio me dar bom dia dei logo um chutão na costela joguei ela na porta e gritei bom dia é o caralho hoje tem evento do #ps5 que mané bom dia acordei pilhadão nessa porra e a ela vem com bom dia toma no cu</t>
+  </si>
+  <si>
+    <t>@rnmgamer93 @zangwlctl nosso ps5 tá garantido 🙆 💍 🙆</t>
+  </si>
+  <si>
+    <t>cria um perfil fake ➡ ️ fala q meus pais me expulsaram de casa pq eu falei q era gay ➡ ️ mendigar ➡ ️ ganha 10 mil ➡ ️ compra o iphone 12 e guarda pro ps5 ✅</t>
+  </si>
+  <si>
+    <t>@carlinhostroll no laçamento do ps4.. comprei de você que ajudou vários gamers brasileiros você podia vender novamente o xbox e ps5 em 🥺</t>
+  </si>
+  <si>
+    <t>já trouxe o terno da lavanderia. pro martini mexido e não batido tem tudo.mandei os cachorros pra casa da vó e as crianças pra pet 🤔 🤔 🤔 .pedi divórcio entre 16h45 até 18h45. desfiz todas as amizades.hoje é dia de #ps5showcase #ps5</t>
+  </si>
+  <si>
+    <t>tomara que a rapaziada do xbox n venha pro ps5 tem uns q são chatão pqp</t>
+  </si>
+  <si>
+    <t>jogos que adoraria ver aparecendo amanhã na conferência do ps5 mas que obviamente vão permanecer só nos corações mesmo 😭 👌 https//t.co/5qadryqu7v</t>
   </si>
 </sst>
 </file>
@@ -2882,15 +2909,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C301" sqref="C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="255.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="77.7109375" customWidth="1"/>
+    <col min="3" max="3" width="111.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3165,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>519</v>
+        <v>679</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3176,7 +3203,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3198,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>521</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3209,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3220,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3242,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -3275,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -3286,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>527</v>
+        <v>681</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,7 +3335,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -3341,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>531</v>
+        <v>682</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3352,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3385,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3396,7 +3423,7 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>534</v>
+        <v>683</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3429,7 +3456,7 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>536</v>
+        <v>684</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3440,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>537</v>
+        <v>685</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,7 +3489,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>538</v>
+        <v>686</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3484,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,7 +3555,7 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,7 +3577,7 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -3561,7 +3588,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>687</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3583,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3605,7 +3632,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3616,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3627,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -3638,7 +3665,7 @@
         <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3649,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3682,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3693,7 +3720,7 @@
         <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3704,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -3715,7 +3742,7 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3726,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -3737,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>555</v>
+        <v>688</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3748,7 +3775,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>78</v>
+        <v>689</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3759,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3770,7 +3797,7 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>557</v>
+        <v>690</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -3781,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>558</v>
+        <v>691</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3792,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>559</v>
+        <v>692</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3803,7 +3830,7 @@
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -3814,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3825,7 +3852,7 @@
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -3836,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3858,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3880,7 +3907,7 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -3891,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3902,7 +3929,7 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3913,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -3924,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3935,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3946,7 +3973,7 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3957,7 +3984,7 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3968,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3979,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3990,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -4001,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4012,7 +4039,7 @@
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>577</v>
+        <v>693</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -4023,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -4078,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,7 +4127,7 @@
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>580</v>
+        <v>694</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -4122,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="150" x14ac:dyDescent="0.25">
@@ -4133,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -4155,7 +4182,7 @@
         <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -4166,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,7 +4204,7 @@
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,7 +4215,7 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4199,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>587</v>
+        <v>695</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4210,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -4221,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -4232,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="C122" t="s">
-        <v>590</v>
+        <v>696</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4243,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4254,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>592</v>
+        <v>576</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4276,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="C126" t="s">
-        <v>593</v>
+        <v>577</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -4287,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="C127" t="s">
-        <v>594</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4298,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>595</v>
+        <v>697</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4309,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>596</v>
+        <v>579</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4331,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>597</v>
+        <v>580</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4342,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>598</v>
+        <v>581</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4364,7 +4391,7 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>599</v>
+        <v>698</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -4375,7 +4402,7 @@
         <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="C141" t="s">
-        <v>602</v>
+        <v>699</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4452,7 +4479,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>603</v>
+        <v>584</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,7 +4490,7 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>604</v>
+        <v>585</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4474,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>605</v>
+        <v>586</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4485,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="C145" t="s">
-        <v>606</v>
+        <v>587</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -4507,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="C147" t="s">
-        <v>607</v>
+        <v>588</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4518,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="C148" t="s">
-        <v>608</v>
+        <v>589</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4540,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>609</v>
+        <v>700</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4551,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="C151" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -4562,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -4573,7 +4600,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>612</v>
+        <v>701</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -4595,7 +4622,7 @@
         <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4606,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>614</v>
+        <v>593</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4617,7 +4644,7 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>615</v>
+        <v>702</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4639,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="C159" t="s">
-        <v>616</v>
+        <v>703</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4650,7 +4677,7 @@
         <v>0</v>
       </c>
       <c r="C160" t="s">
-        <v>617</v>
+        <v>594</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4661,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="C161" t="s">
-        <v>618</v>
+        <v>595</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4683,7 +4710,7 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>163</v>
+        <v>704</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4705,7 +4732,7 @@
         <v>0</v>
       </c>
       <c r="C165" t="s">
-        <v>619</v>
+        <v>596</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -4716,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>166</v>
+        <v>705</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4727,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="C167" t="s">
-        <v>620</v>
+        <v>597</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4738,7 +4765,7 @@
         <v>0</v>
       </c>
       <c r="C168" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4749,7 +4776,7 @@
         <v>1</v>
       </c>
       <c r="C169" t="s">
-        <v>622</v>
+        <v>706</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -4782,7 +4809,7 @@
         <v>1</v>
       </c>
       <c r="C172" t="s">
-        <v>172</v>
+        <v>707</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -4793,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="C173" t="s">
-        <v>623</v>
+        <v>599</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4815,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="C175" t="s">
-        <v>624</v>
+        <v>600</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4826,7 +4853,7 @@
         <v>0</v>
       </c>
       <c r="C176" t="s">
-        <v>625</v>
+        <v>601</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4837,7 +4864,7 @@
         <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>626</v>
+        <v>602</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -4848,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="C178" t="s">
-        <v>627</v>
+        <v>708</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4859,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>628</v>
+        <v>603</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4870,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>629</v>
+        <v>604</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4881,7 +4908,7 @@
         <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4892,7 +4919,7 @@
         <v>0</v>
       </c>
       <c r="C182" t="s">
-        <v>631</v>
+        <v>709</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,7 +4930,7 @@
         <v>0</v>
       </c>
       <c r="C183" t="s">
-        <v>632</v>
+        <v>606</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -4914,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="C184" t="s">
-        <v>633</v>
+        <v>607</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4925,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>634</v>
+        <v>608</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -4969,7 +4996,7 @@
         <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>635</v>
+        <v>609</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4980,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="C190" t="s">
-        <v>636</v>
+        <v>610</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4991,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="C191" t="s">
-        <v>637</v>
+        <v>710</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -5002,7 +5029,7 @@
         <v>0</v>
       </c>
       <c r="C192" t="s">
-        <v>638</v>
+        <v>611</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -5013,7 +5040,7 @@
         <v>0</v>
       </c>
       <c r="C193" t="s">
-        <v>639</v>
+        <v>612</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5024,7 +5051,7 @@
         <v>1</v>
       </c>
       <c r="C194" t="s">
-        <v>640</v>
+        <v>711</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -5035,7 +5062,7 @@
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>641</v>
+        <v>613</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -5057,7 +5084,7 @@
         <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>642</v>
+        <v>712</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5068,7 +5095,7 @@
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>643</v>
+        <v>614</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -5079,7 +5106,7 @@
         <v>0</v>
       </c>
       <c r="C199" t="s">
-        <v>644</v>
+        <v>615</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -5101,7 +5128,7 @@
         <v>0</v>
       </c>
       <c r="C201" t="s">
-        <v>645</v>
+        <v>616</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -5112,7 +5139,7 @@
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>646</v>
+        <v>617</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -5123,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="C203" t="s">
-        <v>203</v>
+        <v>713</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -5134,7 +5161,7 @@
         <v>1</v>
       </c>
       <c r="C204" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -5145,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="C205" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5156,7 +5183,7 @@
         <v>1</v>
       </c>
       <c r="C206" t="s">
-        <v>649</v>
+        <v>620</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -5178,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="C208" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -5189,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="C209" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5211,7 +5238,7 @@
         <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>652</v>
+        <v>623</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -5233,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>653</v>
+        <v>624</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -5244,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="C214" t="s">
-        <v>654</v>
+        <v>714</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -5255,7 +5282,7 @@
         <v>0</v>
       </c>
       <c r="C215" t="s">
-        <v>655</v>
+        <v>715</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -5266,7 +5293,7 @@
         <v>1</v>
       </c>
       <c r="C216" t="s">
-        <v>656</v>
+        <v>716</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -5277,7 +5304,7 @@
         <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -5299,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -5310,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="C220" t="s">
-        <v>659</v>
+        <v>627</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -5321,7 +5348,7 @@
         <v>0</v>
       </c>
       <c r="C221" t="s">
-        <v>660</v>
+        <v>628</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -5332,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="C222" t="s">
-        <v>661</v>
+        <v>717</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -5343,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="C223" t="s">
-        <v>662</v>
+        <v>629</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -5365,7 +5392,7 @@
         <v>0</v>
       </c>
       <c r="C225" t="s">
-        <v>663</v>
+        <v>630</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -5376,7 +5403,7 @@
         <v>1</v>
       </c>
       <c r="C226" t="s">
-        <v>664</v>
+        <v>631</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -5387,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="C227" t="s">
-        <v>665</v>
+        <v>632</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -5398,7 +5425,7 @@
         <v>1</v>
       </c>
       <c r="C228" t="s">
-        <v>228</v>
+        <v>718</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -5420,7 +5447,7 @@
         <v>0</v>
       </c>
       <c r="C230" t="s">
-        <v>666</v>
+        <v>633</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="210" x14ac:dyDescent="0.25">
@@ -5431,7 +5458,7 @@
         <v>1</v>
       </c>
       <c r="C231" t="s">
-        <v>667</v>
+        <v>634</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -5442,7 +5469,7 @@
         <v>1</v>
       </c>
       <c r="C232" t="s">
-        <v>668</v>
+        <v>635</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5453,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="C233" t="s">
-        <v>669</v>
+        <v>719</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5464,7 +5491,7 @@
         <v>0</v>
       </c>
       <c r="C234" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -5486,7 +5513,7 @@
         <v>1</v>
       </c>
       <c r="C236" t="s">
-        <v>671</v>
+        <v>637</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -5497,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="C237" t="s">
-        <v>672</v>
+        <v>638</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -5508,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="C238" t="s">
-        <v>673</v>
+        <v>720</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -5519,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="C239" t="s">
-        <v>674</v>
+        <v>721</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5530,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="C240" t="s">
-        <v>675</v>
+        <v>639</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -5541,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="C241" t="s">
-        <v>676</v>
+        <v>640</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -5552,7 +5579,7 @@
         <v>1</v>
       </c>
       <c r="C242" t="s">
-        <v>677</v>
+        <v>641</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5563,7 +5590,7 @@
         <v>1</v>
       </c>
       <c r="C243" t="s">
-        <v>678</v>
+        <v>642</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -5585,7 +5612,7 @@
         <v>1</v>
       </c>
       <c r="C245" t="s">
-        <v>679</v>
+        <v>643</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5596,7 +5623,7 @@
         <v>1</v>
       </c>
       <c r="C246" t="s">
-        <v>680</v>
+        <v>644</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -5607,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="C247" t="s">
-        <v>681</v>
+        <v>645</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -5618,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="C248" t="s">
-        <v>682</v>
+        <v>722</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -5629,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="C249" t="s">
-        <v>683</v>
+        <v>646</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -5640,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="C250" t="s">
-        <v>684</v>
+        <v>647</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -5662,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="C252" t="s">
-        <v>685</v>
+        <v>648</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -5684,7 +5711,7 @@
         <v>0</v>
       </c>
       <c r="C254" t="s">
-        <v>686</v>
+        <v>649</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -5695,7 +5722,7 @@
         <v>0</v>
       </c>
       <c r="C255" t="s">
-        <v>687</v>
+        <v>650</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -5706,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="C256" t="s">
-        <v>688</v>
+        <v>651</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -5717,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="C257" t="s">
-        <v>689</v>
+        <v>652</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -5728,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="C258" t="s">
-        <v>690</v>
+        <v>653</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,7 +5766,7 @@
         <v>0</v>
       </c>
       <c r="C259" t="s">
-        <v>259</v>
+        <v>723</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5750,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="C260" t="s">
-        <v>691</v>
+        <v>654</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -5761,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="C261" t="s">
-        <v>692</v>
+        <v>655</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -5783,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="C263" t="s">
-        <v>693</v>
+        <v>656</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -5805,7 +5832,7 @@
         <v>0</v>
       </c>
       <c r="C265" t="s">
-        <v>694</v>
+        <v>657</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -5827,7 +5854,7 @@
         <v>0</v>
       </c>
       <c r="C267" t="s">
-        <v>695</v>
+        <v>658</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5838,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="C268" t="s">
-        <v>696</v>
+        <v>659</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -5871,7 +5898,7 @@
         <v>1</v>
       </c>
       <c r="C271" t="s">
-        <v>697</v>
+        <v>660</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -5882,7 +5909,7 @@
         <v>0</v>
       </c>
       <c r="C272" t="s">
-        <v>272</v>
+        <v>724</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -5893,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="C273" t="s">
-        <v>698</v>
+        <v>661</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5904,7 +5931,7 @@
         <v>1</v>
       </c>
       <c r="C274" t="s">
-        <v>699</v>
+        <v>662</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5926,7 +5953,7 @@
         <v>1</v>
       </c>
       <c r="C276" t="s">
-        <v>700</v>
+        <v>663</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5937,7 +5964,7 @@
         <v>1</v>
       </c>
       <c r="C277" t="s">
-        <v>701</v>
+        <v>664</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -5948,7 +5975,7 @@
         <v>1</v>
       </c>
       <c r="C278" t="s">
-        <v>702</v>
+        <v>665</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5959,7 +5986,7 @@
         <v>0</v>
       </c>
       <c r="C279" t="s">
-        <v>703</v>
+        <v>666</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5970,7 +5997,7 @@
         <v>1</v>
       </c>
       <c r="C280" t="s">
-        <v>704</v>
+        <v>667</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -5992,7 +6019,7 @@
         <v>0</v>
       </c>
       <c r="C282" t="s">
-        <v>705</v>
+        <v>725</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -6003,7 +6030,7 @@
         <v>0</v>
       </c>
       <c r="C283" t="s">
-        <v>706</v>
+        <v>726</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -6025,7 +6052,7 @@
         <v>1</v>
       </c>
       <c r="C285" t="s">
-        <v>707</v>
+        <v>668</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -6036,7 +6063,7 @@
         <v>1</v>
       </c>
       <c r="C286" t="s">
-        <v>708</v>
+        <v>727</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -6047,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="C287" t="s">
-        <v>709</v>
+        <v>728</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -6069,7 +6096,7 @@
         <v>1</v>
       </c>
       <c r="C289" t="s">
-        <v>710</v>
+        <v>669</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -6091,7 +6118,7 @@
         <v>1</v>
       </c>
       <c r="C291" t="s">
-        <v>711</v>
+        <v>670</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -6102,7 +6129,7 @@
         <v>0</v>
       </c>
       <c r="C292" t="s">
-        <v>712</v>
+        <v>671</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -6113,7 +6140,7 @@
         <v>0</v>
       </c>
       <c r="C293" t="s">
-        <v>713</v>
+        <v>672</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -6146,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="C296" t="s">
-        <v>714</v>
+        <v>673</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -6157,7 +6184,7 @@
         <v>0</v>
       </c>
       <c r="C297" t="s">
-        <v>715</v>
+        <v>674</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -6168,7 +6195,7 @@
         <v>0</v>
       </c>
       <c r="C298" t="s">
-        <v>716</v>
+        <v>675</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -6179,7 +6206,7 @@
         <v>0</v>
       </c>
       <c r="C299" t="s">
-        <v>717</v>
+        <v>676</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -6190,7 +6217,7 @@
         <v>0</v>
       </c>
       <c r="C300" t="s">
-        <v>718</v>
+        <v>677</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -6201,7 +6228,7 @@
         <v>1</v>
       </c>
       <c r="C301" t="s">
-        <v>719</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Classificador implementado (fazer correcoes)
</commit_message>
<xml_diff>
--- a/PS5.xlsx
+++ b/PS5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agchi\Documents\GitHub\P1-Ciencia-dos-Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99AB76-F88C-4CA7-AD99-54FBC1F20616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33C45AD-9FE9-4C3B-BAF8-8D80E52CCC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4635" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2909,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2958,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>505</v>
@@ -3200,7 +3200,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>519</v>
@@ -3376,7 +3376,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
         <v>528</v>

</xml_diff>